<commit_message>
[project] Documentaion and other amendments
 - examples in data documentation
 - example analysis
</commit_message>
<xml_diff>
--- a/data-raw/ucs_lus.xlsx
+++ b/data-raw/ucs_lus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DE97214F-2E7E-45C0-AA15-FA2D2AAF6FF0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B130DF78-9D22-436F-B446-8E7C2D182A50}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="13095" windowHeight="7770" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="13095" windowHeight="7770" tabRatio="699" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="HTML_PathFile" hidden="1">"G:\ACTIVITY\HELP\DTPANIC\2001-02\MyHTML.htm"</definedName>
     <definedName name="HTML_Title" hidden="1">"Section 1"</definedName>
   </definedNames>
-  <calcPr calcId="179017" calcMode="manual"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -185,9 +185,6 @@
     <t>I8[0-2]</t>
   </si>
   <si>
-    <t>E1[0-5];E16[12]</t>
-  </si>
-  <si>
     <t>G4[01]</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>UCS conditions as specified in CCG IAF 201617</t>
+  </si>
+  <si>
+    <t>E1[0-5]|E16[12]</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1500,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f ca="1">TODAY()</f>
-        <v>43536</v>
+        <v>43539</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1603,7 +1603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F526BF-D9A6-4A08-87CA-ADC99D6ACA94}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1613,7 +1615,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1767,7 +1769,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1809,7 +1811,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1840,24 +1842,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0507C8F2-EB71-414F-87E6-7CCD0F976961}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
[project] Adapt uc for no version in conditions.
</commit_message>
<xml_diff>
--- a/data-raw/ucs_lus.xlsx
+++ b/data-raw/ucs_lus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B130DF78-9D22-436F-B446-8E7C2D182A50}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37B37711-0697-45A4-A2B0-F36A132821C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="13095" windowHeight="7770" tabRatio="699" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Prepared by:</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>E1[0-5]|E16[12]</t>
+  </si>
+  <si>
+    <t>cat1</t>
+  </si>
+  <si>
+    <t>cat2</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,23 @@
     <cellStyle name="Normal 5 2" xfId="6" xr:uid="{E757CAE4-A39C-4AE3-95B2-8A65678088A1}"/>
     <cellStyle name="Normal 6 2 2" xfId="4" xr:uid="{B0B1FA75-ACA4-424E-8D9B-3DC7352572AB}"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -804,42 +829,42 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="NCC White Table" defaultPivotStyle="NCC White Pivot">
     <tableStyle name="NCC White Pivot" table="0" count="11" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="36"/>
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="totalRow" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="31"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="30"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="29"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="28"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="27"/>
-      <tableStyleElement type="pageFieldValues" dxfId="26"/>
+      <tableStyleElement type="wholeTable" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="37"/>
+      <tableStyleElement type="totalRow" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="34"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="33"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="32"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="31"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="30"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="29"/>
+      <tableStyleElement type="pageFieldValues" dxfId="28"/>
     </tableStyle>
     <tableStyle name="NCC White Table" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="firstColumn" dxfId="22"/>
-      <tableStyleElement type="lastColumn" dxfId="21"/>
-      <tableStyleElement type="firstRowStripe" dxfId="20"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="totalRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
+      <tableStyleElement type="lastColumn" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="21"/>
     </tableStyle>
     <tableStyle name="PivotNCCDefaultBlue" table="0" count="14" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="totalRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="14"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="secondColumnSubheading" dxfId="10"/>
-      <tableStyleElement type="thirdColumnSubheading" dxfId="9"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="8"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="7"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="6"/>
-      <tableStyleElement type="pageFieldValues" dxfId="5"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
+      <tableStyleElement type="secondColumnSubheading" dxfId="12"/>
+      <tableStyleElement type="thirdColumnSubheading" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1133,26 +1158,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E22A2325-3E08-4CDD-B40F-7E0B52F68F7E}" name="Table2" displayName="Table2" ref="A3:D17" totalsRowShown="0">
-  <autoFilter ref="A3:D17" xr:uid="{12F0A6E3-9939-4F36-9F23-9E566736150C}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E22A2325-3E08-4CDD-B40F-7E0B52F68F7E}" name="Table2" displayName="Table2" ref="A3:F17" totalsRowShown="0">
+  <autoFilter ref="A3:F17" xr:uid="{12F0A6E3-9939-4F36-9F23-9E566736150C}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E00B5BA3-1660-4ACA-BD4D-87910B07DA6B}" name="Condition description"/>
     <tableColumn id="2" xr3:uid="{BD7E279D-637E-4828-970E-BB2161792735}" name="primary diagnosis"/>
     <tableColumn id="3" xr3:uid="{9E6F3A78-DE07-4BCE-8881-CD1A109A947D}" name="age"/>
     <tableColumn id="4" xr3:uid="{9306E100-50CC-4A6B-85CD-B0F1BAACD48F}" name="primary_regex"/>
+    <tableColumn id="5" xr3:uid="{0F41B8B5-0C11-49BF-ACEA-BCAFD1DADD62}" name="cat1" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{4D31A873-BBD1-4486-9ABC-7545D1E1F762}" name="cat2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="NCC White Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D363AFF-0684-4EE3-A4E0-FA1E0BDD936B}" name="Table1" displayName="Table1" ref="A3:D6" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D363AFF-0684-4EE3-A4E0-FA1E0BDD936B}" name="Table1" displayName="Table1" ref="A3:D6" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A3:D6" xr:uid="{4313B3E6-31BC-4763-B1FF-DBE83183C343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{27384D85-459D-4810-88D9-4E9978105AC1}" name="ab_ucs" dataDxfId="3" dataCellStyle="Normal 5 2"/>
-    <tableColumn id="2" xr3:uid="{F8899CCC-54AB-4D06-95D5-B5FC087E819A}" name="0 - 5 yrs" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{D50CDBFE-824E-47F5-9DD6-94F512E32591}" name="6 - 74 yrs" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B036D52A-0567-4117-9173-51FE69D79327}" name="75+ yrs" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{27384D85-459D-4810-88D9-4E9978105AC1}" name="ab_ucs" dataDxfId="5" dataCellStyle="Normal 5 2"/>
+    <tableColumn id="2" xr3:uid="{F8899CCC-54AB-4D06-95D5-B5FC087E819A}" name="0 - 5 yrs" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D50CDBFE-824E-47F5-9DD6-94F512E32591}" name="6 - 74 yrs" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B036D52A-0567-4117-9173-51FE69D79327}" name="75+ yrs" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="NCC White Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1500,7 +1527,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f ca="1">TODAY()</f>
-        <v>43539</v>
+        <v>43542</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1601,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F526BF-D9A6-4A08-87CA-ADC99D6ACA94}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1613,12 +1640,12 @@
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1631,8 +1658,14 @@
       <c r="D3" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1645,8 +1678,14 @@
       <c r="D4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1659,8 +1698,14 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1673,8 +1718,14 @@
       <c r="D6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1687,8 +1738,14 @@
       <c r="D7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1701,8 +1758,14 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1715,8 +1778,14 @@
       <c r="D9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1729,8 +1798,14 @@
       <c r="D10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1743,8 +1818,14 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1757,8 +1838,14 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1771,8 +1858,14 @@
       <c r="D13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1785,8 +1878,14 @@
       <c r="D14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1799,8 +1898,14 @@
       <c r="D15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1813,8 +1918,14 @@
       <c r="D16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1826,6 +1937,12 @@
       </c>
       <c r="D17" t="s">
         <v>39</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>